<commit_message>
create BU and respective teams completed
</commit_message>
<xml_diff>
--- a/dataCenter.xlsx
+++ b/dataCenter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe.cacho\Documents\MY  CODE\CrmHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CEF049-0EB7-48E5-8A15-84BFFD1316D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7AF7FF-83CC-4F1C-81A7-1FEED12F6CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DF524610-1964-40D8-A05C-F2A29F859B9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF524610-1964-40D8-A05C-F2A29F859B9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Teams" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>BU</t>
   </si>
@@ -60,15 +60,6 @@
     <t>Team To Assign</t>
   </si>
   <si>
-    <t>0-PT-BDR-01</t>
-  </si>
-  <si>
-    <t>OMNINSTAL</t>
-  </si>
-  <si>
-    <t>ESOE0033</t>
-  </si>
-  <si>
     <t>ZPQ</t>
   </si>
   <si>
@@ -79,6 +70,18 @@
   </si>
   <si>
     <t>EX152690</t>
+  </si>
+  <si>
+    <t>T501</t>
+  </si>
+  <si>
+    <t>GAMESA</t>
+  </si>
+  <si>
+    <t>ETGA0001</t>
+  </si>
+  <si>
+    <t>0-ES-BRJ-07</t>
   </si>
 </sst>
 </file>
@@ -488,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587A5E4A-68E0-4D45-BDD1-D8521CA067EB}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,19 +524,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2100</v>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -545,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD2AA51F-8547-4986-84C6-C90D78884D49}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -568,18 +571,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added NAS massive download folder organizer
working prototype with hardcoded query that organizes the files, you need to select the folder where the unorganized files are
</commit_message>
<xml_diff>
--- a/dataCenter.xlsx
+++ b/dataCenter.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe.cacho\Documents\MY  CODE\CrmHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7AF7FF-83CC-4F1C-81A7-1FEED12F6CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A20F1E8-FFA0-4C6F-9131-DE4103363C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF524610-1964-40D8-A05C-F2A29F859B9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DF524610-1964-40D8-A05C-F2A29F859B9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Teams" sheetId="3" r:id="rId1"/>
-    <sheet name="Assign Teams" sheetId="4" r:id="rId2"/>
+    <sheet name="NAS Downloads" sheetId="5" r:id="rId2"/>
+    <sheet name="Assign Teams" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>BU</t>
   </si>
@@ -82,6 +83,15 @@
   </si>
   <si>
     <t>0-ES-BRJ-07</t>
+  </si>
+  <si>
+    <t>Functional Location (level 3)</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>0-FR-BBC</t>
   </si>
 </sst>
 </file>
@@ -137,7 +147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,6 +163,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -491,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587A5E4A-68E0-4D45-BDD1-D8521CA067EB}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -545,12 +558,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8125D225-87DB-4514-B520-D59F3D484DA4}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2024</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD2AA51F-8547-4986-84C6-C90D78884D49}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
fixed extract users from teams and removed park visualizer
park visualizer might return at a later date but for now it doesn't make sense to keep it when its not working
</commit_message>
<xml_diff>
--- a/dataCenter.xlsx
+++ b/dataCenter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe.cacho\Documents\MY  CODE\CrmHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE09FFE-AFA8-42B3-A142-ECA55B674328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35716BA3-9083-403D-B4C9-B824FA8957EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{DF524610-1964-40D8-A05C-F2A29F859B9B}"/>
+    <workbookView xWindow="4200" yWindow="1365" windowWidth="21600" windowHeight="11295" xr2:uid="{DF524610-1964-40D8-A05C-F2A29F859B9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Teams" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>BU</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Team To Assign</t>
   </si>
   <si>
-    <t>ZPQ</t>
-  </si>
-  <si>
     <t>Equipo contrata 0-ES-ACA-01</t>
   </si>
   <si>
@@ -73,18 +70,6 @@
     <t>EX152690</t>
   </si>
   <si>
-    <t>T501</t>
-  </si>
-  <si>
-    <t>GAMESA</t>
-  </si>
-  <si>
-    <t>ETGA0001</t>
-  </si>
-  <si>
-    <t>0-ES-BRJ-07</t>
-  </si>
-  <si>
     <t>Functional Location (level 3)</t>
   </si>
   <si>
@@ -122,6 +107,39 @@
   </si>
   <si>
     <t>0-FR-VDN</t>
+  </si>
+  <si>
+    <t>0-IT-CTL-01</t>
+  </si>
+  <si>
+    <t>EBBK0001</t>
+  </si>
+  <si>
+    <t>ZP1</t>
+  </si>
+  <si>
+    <t>I801</t>
+  </si>
+  <si>
+    <t>BKW</t>
+  </si>
+  <si>
+    <t>0-IT-CTL-02</t>
+  </si>
+  <si>
+    <t>0-IT-VLC-01</t>
+  </si>
+  <si>
+    <t>804I</t>
+  </si>
+  <si>
+    <t>0-IT-BZI-01</t>
+  </si>
+  <si>
+    <t>ETBK0001</t>
+  </si>
+  <si>
+    <t>I810</t>
   </si>
 </sst>
 </file>
@@ -532,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587A5E4A-68E0-4D45-BDD1-D8521CA067EB}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,19 +585,70 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -591,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8125D225-87DB-4514-B520-D59F3D484DA4}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,68 +673,68 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -698,18 +767,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed new assigned team to user
</commit_message>
<xml_diff>
--- a/dataCenter.xlsx
+++ b/dataCenter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe.cacho\Documents\MY  CODE\CrmHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe.cacho\Documents\MYCODE\CrmHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2B61C6-7012-45FF-AFE7-096576272901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7BDE63-C6FF-45F7-A389-ABC27B63D236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF524610-1964-40D8-A05C-F2A29F859B9B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>BU</t>
   </si>
@@ -112,16 +112,22 @@
     <t>ZP1</t>
   </si>
   <si>
-    <t>0-BR-MVS-02</t>
-  </si>
-  <si>
-    <t>EPVL0001</t>
-  </si>
-  <si>
-    <t>3R71</t>
-  </si>
-  <si>
-    <t>VOLTALIA</t>
+    <t>0-ES-BEL-01</t>
+  </si>
+  <si>
+    <t>ETVT0001</t>
+  </si>
+  <si>
+    <t>H314</t>
+  </si>
+  <si>
+    <t>VESTAS</t>
+  </si>
+  <si>
+    <t>0-ES-ACA-01</t>
+  </si>
+  <si>
+    <t>T558</t>
   </si>
 </sst>
 </file>
@@ -532,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587A5E4A-68E0-4D45-BDD1-D8521CA067EB}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,6 +585,23 @@
         <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed assign and remove teams from user when creating new work posts
the code handled the cases correctly where the planner group was zp1 but not when was zpx, it kept forgetting the planner group and the subsquent logic was wrong, it's fixed now
</commit_message>
<xml_diff>
--- a/dataCenter.xlsx
+++ b/dataCenter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe.cacho\Documents\MYCODE\CrmHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7BDE63-C6FF-45F7-A389-ABC27B63D236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBDCBB6-5795-410A-9B44-12F7A5283237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF524610-1964-40D8-A05C-F2A29F859B9B}"/>
+    <workbookView xWindow="4620" yWindow="3930" windowWidth="21600" windowHeight="11295" xr2:uid="{DF524610-1964-40D8-A05C-F2A29F859B9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Teams" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>BU</t>
   </si>
@@ -109,25 +109,22 @@
     <t>0-FR-VDN</t>
   </si>
   <si>
-    <t>ZP1</t>
-  </si>
-  <si>
-    <t>0-ES-BEL-01</t>
-  </si>
-  <si>
-    <t>ETVT0001</t>
-  </si>
-  <si>
-    <t>H314</t>
-  </si>
-  <si>
-    <t>VESTAS</t>
-  </si>
-  <si>
-    <t>0-ES-ACA-01</t>
-  </si>
-  <si>
-    <t>T558</t>
+    <t>0-BR-CEN-01</t>
+  </si>
+  <si>
+    <t>ETIN0001</t>
+  </si>
+  <si>
+    <t>ZPQ</t>
+  </si>
+  <si>
+    <t>B020</t>
+  </si>
+  <si>
+    <t>0-BR-CEN-02</t>
+  </si>
+  <si>
+    <t>PREDIRE</t>
   </si>
 </sst>
 </file>
@@ -541,7 +538,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +547,7 @@
     <col min="2" max="2" width="32.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="41" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -573,36 +570,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>